<commit_message>
Begin data wrangling, and putting together list of species with standardized codes. Move output of 01_curate-species-list.R script to the data/raw/ folder.
</commit_message>
<xml_diff>
--- a/data/raw/master-seed-mix.xlsx
+++ b/data/raw/master-seed-mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405F4FFE-791A-4C0C-A1D8-284F8E4351B4}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BB0CEDC-F36C-4643-A749-1E5E908F71E4}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21624" windowHeight="11112" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="235">
   <si>
     <t>Family</t>
   </si>
@@ -741,9 +741,6 @@
   </si>
   <si>
     <t>Region</t>
-  </si>
-  <si>
-    <t>Native</t>
   </si>
 </sst>
 </file>
@@ -1099,11 +1096,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ED48DE-F67E-409C-BADB-8346B0730F99}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I98"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,7 +1113,7 @@
     <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>234</v>
       </c>
@@ -1141,11 +1138,8 @@
       <c r="H1" t="s">
         <v>229</v>
       </c>
-      <c r="I1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>230</v>
       </c>
@@ -1170,11 +1164,8 @@
       <c r="H2">
         <v>16.25</v>
       </c>
-      <c r="I2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -1199,11 +1190,8 @@
       <c r="H3">
         <v>17.72</v>
       </c>
-      <c r="I3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -1228,11 +1216,8 @@
       <c r="H4">
         <v>17.97</v>
       </c>
-      <c r="I4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -1257,11 +1242,8 @@
       <c r="H5">
         <v>18.63</v>
       </c>
-      <c r="I5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -1286,11 +1268,8 @@
       <c r="H6">
         <v>19.399999999999999</v>
       </c>
-      <c r="I6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>230</v>
       </c>
@@ -1315,11 +1294,8 @@
       <c r="H7">
         <v>15.8</v>
       </c>
-      <c r="I7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>230</v>
       </c>
@@ -1344,11 +1320,8 @@
       <c r="H8">
         <v>19.899999999999999</v>
       </c>
-      <c r="I8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -1373,11 +1346,8 @@
       <c r="H9">
         <v>19.899999999999999</v>
       </c>
-      <c r="I9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>230</v>
       </c>
@@ -1402,11 +1372,8 @@
       <c r="H10">
         <v>20.3</v>
       </c>
-      <c r="I10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>230</v>
       </c>
@@ -1431,11 +1398,8 @@
       <c r="H11">
         <v>20.5</v>
       </c>
-      <c r="I11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>230</v>
       </c>
@@ -1460,11 +1424,8 @@
       <c r="H12">
         <v>21.6</v>
       </c>
-      <c r="I12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -1489,11 +1450,8 @@
       <c r="H13">
         <v>21.84</v>
       </c>
-      <c r="I13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>230</v>
       </c>
@@ -1518,11 +1476,8 @@
       <c r="H14">
         <v>22.5</v>
       </c>
-      <c r="I14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -1547,11 +1502,8 @@
       <c r="H15">
         <v>23.15</v>
       </c>
-      <c r="I15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>230</v>
       </c>
@@ -1576,11 +1528,8 @@
       <c r="H16">
         <v>11.5</v>
       </c>
-      <c r="I16" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>230</v>
       </c>
@@ -1605,11 +1554,8 @@
       <c r="H17">
         <v>14.2</v>
       </c>
-      <c r="I17" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>230</v>
       </c>
@@ -1634,11 +1580,8 @@
       <c r="H18">
         <v>14.2</v>
       </c>
-      <c r="I18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -1663,11 +1606,8 @@
       <c r="H19">
         <v>15.5</v>
       </c>
-      <c r="I19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>230</v>
       </c>
@@ -1692,11 +1632,8 @@
       <c r="H20">
         <v>15.8</v>
       </c>
-      <c r="I20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>230</v>
       </c>
@@ -1721,11 +1658,8 @@
       <c r="H21">
         <v>15.95</v>
       </c>
-      <c r="I21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>230</v>
       </c>
@@ -1750,11 +1684,8 @@
       <c r="H22">
         <v>16</v>
       </c>
-      <c r="I22" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1779,11 +1710,8 @@
       <c r="H23">
         <v>11.4</v>
       </c>
-      <c r="I23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -1808,11 +1736,8 @@
       <c r="H24">
         <v>11.7</v>
       </c>
-      <c r="I24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1837,11 +1762,8 @@
       <c r="H25">
         <v>12</v>
       </c>
-      <c r="I25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1866,11 +1788,8 @@
       <c r="H26">
         <v>12.1</v>
       </c>
-      <c r="I26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1895,11 +1814,8 @@
       <c r="H27">
         <v>12.7</v>
       </c>
-      <c r="I27" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1924,11 +1840,8 @@
       <c r="H28">
         <v>14.2</v>
       </c>
-      <c r="I28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1950,11 +1863,8 @@
       <c r="G29">
         <v>14</v>
       </c>
-      <c r="I29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1979,11 +1889,8 @@
       <c r="H30">
         <v>13.3</v>
       </c>
-      <c r="I30" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -2008,11 +1915,8 @@
       <c r="H31">
         <v>13.7</v>
       </c>
-      <c r="I31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2037,11 +1941,8 @@
       <c r="H32">
         <v>14.2</v>
       </c>
-      <c r="I32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -2066,11 +1967,8 @@
       <c r="H33">
         <v>15.5</v>
       </c>
-      <c r="I33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2095,11 +1993,8 @@
       <c r="H34">
         <v>15.5</v>
       </c>
-      <c r="I34" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2124,11 +2019,8 @@
       <c r="H35">
         <v>15.7</v>
       </c>
-      <c r="I35" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2153,11 +2045,8 @@
       <c r="H36">
         <v>15.9</v>
       </c>
-      <c r="I36" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2182,11 +2071,8 @@
       <c r="H37">
         <v>15.1</v>
       </c>
-      <c r="I37" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2211,11 +2097,8 @@
       <c r="H38">
         <v>16.7</v>
       </c>
-      <c r="I38" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2240,11 +2123,8 @@
       <c r="H39">
         <v>16.899999999999999</v>
       </c>
-      <c r="I39" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2269,11 +2149,8 @@
       <c r="H40">
         <v>17</v>
       </c>
-      <c r="I40" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -2298,11 +2175,8 @@
       <c r="H41">
         <v>17.100000000000001</v>
       </c>
-      <c r="I41" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2327,11 +2201,8 @@
       <c r="H42">
         <v>17.399999999999999</v>
       </c>
-      <c r="I42" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2356,11 +2227,8 @@
       <c r="H43">
         <v>18.100000000000001</v>
       </c>
-      <c r="I43" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -2382,11 +2250,8 @@
       <c r="G44">
         <v>3</v>
       </c>
-      <c r="I44" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -2411,11 +2276,8 @@
       <c r="H45">
         <v>18.3</v>
       </c>
-      <c r="I45" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -2440,11 +2302,8 @@
       <c r="H46">
         <v>18.7</v>
       </c>
-      <c r="I46" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -2469,11 +2328,8 @@
       <c r="H47">
         <v>19.399999999999999</v>
       </c>
-      <c r="I47" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -2498,11 +2354,8 @@
       <c r="H48">
         <v>21.1</v>
       </c>
-      <c r="I48" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -2527,11 +2380,8 @@
       <c r="H49">
         <v>21.4</v>
       </c>
-      <c r="I49" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -2556,11 +2406,8 @@
       <c r="H50">
         <v>21.5</v>
       </c>
-      <c r="I50" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -2585,11 +2432,8 @@
       <c r="H51">
         <v>21.7</v>
       </c>
-      <c r="I51" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2614,11 +2458,8 @@
       <c r="H52">
         <v>21.6</v>
       </c>
-      <c r="I52" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>231</v>
       </c>
@@ -2643,11 +2484,8 @@
       <c r="H53">
         <v>17.97</v>
       </c>
-      <c r="I53" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>231</v>
       </c>
@@ -2672,11 +2510,8 @@
       <c r="H54">
         <v>20.25</v>
       </c>
-      <c r="I54" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -2701,11 +2536,8 @@
       <c r="H55">
         <v>19.86</v>
       </c>
-      <c r="I55" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -2730,11 +2562,8 @@
       <c r="H56">
         <v>21.84</v>
       </c>
-      <c r="I56" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>231</v>
       </c>
@@ -2759,11 +2588,8 @@
       <c r="H57">
         <v>21.94</v>
       </c>
-      <c r="I57" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>231</v>
       </c>
@@ -2788,11 +2614,8 @@
       <c r="H58">
         <v>23.31</v>
       </c>
-      <c r="I58" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>231</v>
       </c>
@@ -2817,11 +2640,8 @@
       <c r="H59">
         <v>20.25</v>
       </c>
-      <c r="I59" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -2843,11 +2663,8 @@
       <c r="G60">
         <v>1</v>
       </c>
-      <c r="I60" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>231</v>
       </c>
@@ -2872,11 +2689,8 @@
       <c r="H61">
         <v>22.5</v>
       </c>
-      <c r="I61" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>231</v>
       </c>
@@ -2901,11 +2715,8 @@
       <c r="H62">
         <v>22.96</v>
       </c>
-      <c r="I62" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>231</v>
       </c>
@@ -2930,11 +2741,8 @@
       <c r="H63">
         <v>23.18</v>
       </c>
-      <c r="I63" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>231</v>
       </c>
@@ -2959,11 +2767,8 @@
       <c r="H64">
         <v>23.33</v>
       </c>
-      <c r="I64" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>231</v>
       </c>
@@ -2988,11 +2793,8 @@
       <c r="H65">
         <v>23.38</v>
       </c>
-      <c r="I65" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>231</v>
       </c>
@@ -3017,11 +2819,8 @@
       <c r="H66">
         <v>23.38</v>
       </c>
-      <c r="I66" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -3046,11 +2845,8 @@
       <c r="H67">
         <v>23.52</v>
       </c>
-      <c r="I67" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -3072,11 +2868,8 @@
       <c r="G68">
         <v>2</v>
       </c>
-      <c r="I68" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -3101,11 +2894,8 @@
       <c r="H69">
         <v>13.7</v>
       </c>
-      <c r="I69" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>232</v>
       </c>
@@ -3130,11 +2920,8 @@
       <c r="H70">
         <v>16.25</v>
       </c>
-      <c r="I70" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>232</v>
       </c>
@@ -3159,11 +2946,8 @@
       <c r="H71">
         <v>16.7</v>
       </c>
-      <c r="I71" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>232</v>
       </c>
@@ -3188,11 +2972,8 @@
       <c r="H72">
         <v>17.97</v>
       </c>
-      <c r="I72" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>232</v>
       </c>
@@ -3217,11 +2998,8 @@
       <c r="H73">
         <v>18.63</v>
       </c>
-      <c r="I73" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>232</v>
       </c>
@@ -3246,11 +3024,8 @@
       <c r="H74">
         <v>19.399999999999999</v>
       </c>
-      <c r="I74" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>232</v>
       </c>
@@ -3272,11 +3047,8 @@
       <c r="G75">
         <v>3</v>
       </c>
-      <c r="I75" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>232</v>
       </c>
@@ -3301,11 +3073,8 @@
       <c r="H76">
         <v>15.97</v>
       </c>
-      <c r="I76" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>232</v>
       </c>
@@ -3330,11 +3099,8 @@
       <c r="H77">
         <v>18.100000000000001</v>
       </c>
-      <c r="I77" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>232</v>
       </c>
@@ -3359,11 +3125,8 @@
       <c r="H78">
         <v>19.399999999999999</v>
       </c>
-      <c r="I78" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>232</v>
       </c>
@@ -3388,11 +3151,8 @@
       <c r="H79">
         <v>21.1</v>
       </c>
-      <c r="I79" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>232</v>
       </c>
@@ -3417,11 +3177,8 @@
       <c r="H80">
         <v>21.7</v>
       </c>
-      <c r="I80" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>232</v>
       </c>
@@ -3446,11 +3203,8 @@
       <c r="H81">
         <v>21.84</v>
       </c>
-      <c r="I81" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -3475,11 +3229,8 @@
       <c r="H82">
         <v>23.15</v>
       </c>
-      <c r="I82" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>233</v>
       </c>
@@ -3504,11 +3255,8 @@
       <c r="H83">
         <v>19.399999999999999</v>
       </c>
-      <c r="I83" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>233</v>
       </c>
@@ -3533,11 +3281,8 @@
       <c r="H84">
         <v>21.84</v>
       </c>
-      <c r="I84" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>233</v>
       </c>
@@ -3562,11 +3307,8 @@
       <c r="H85">
         <v>22.96</v>
       </c>
-      <c r="I85" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>233</v>
       </c>
@@ -3591,11 +3333,8 @@
       <c r="H86">
         <v>22.89</v>
       </c>
-      <c r="I86" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>233</v>
       </c>
@@ -3620,11 +3359,8 @@
       <c r="H87">
         <v>22.87</v>
       </c>
-      <c r="I87" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>233</v>
       </c>
@@ -3649,11 +3385,8 @@
       <c r="H88">
         <v>21.75</v>
       </c>
-      <c r="I88" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>233</v>
       </c>
@@ -3678,11 +3411,8 @@
       <c r="H89">
         <v>20.86</v>
       </c>
-      <c r="I89" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>233</v>
       </c>
@@ -3707,11 +3437,8 @@
       <c r="H90">
         <v>21.66</v>
       </c>
-      <c r="I90" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>233</v>
       </c>
@@ -3736,11 +3463,8 @@
       <c r="H91">
         <v>23.46</v>
       </c>
-      <c r="I91" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>233</v>
       </c>
@@ -3765,11 +3489,8 @@
       <c r="H92">
         <v>23.15</v>
       </c>
-      <c r="I92" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>233</v>
       </c>
@@ -3794,11 +3515,8 @@
       <c r="H93">
         <v>23.38</v>
       </c>
-      <c r="I93" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>233</v>
       </c>
@@ -3823,11 +3541,8 @@
       <c r="H94">
         <v>23.97</v>
       </c>
-      <c r="I94" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -3852,11 +3567,8 @@
       <c r="H95">
         <v>23.5</v>
       </c>
-      <c r="I95" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>233</v>
       </c>
@@ -3881,11 +3593,8 @@
       <c r="H96">
         <v>23.83</v>
       </c>
-      <c r="I96" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>233</v>
       </c>
@@ -3910,11 +3619,8 @@
       <c r="H97">
         <v>24.88</v>
       </c>
-      <c r="I97" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>233</v>
       </c>
@@ -3938,9 +3644,6 @@
       </c>
       <c r="H98">
         <v>24.2</v>
-      </c>
-      <c r="I98" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrambled to put together some TRY stuff and finished editing 2x2 species list
</commit_message>
<xml_diff>
--- a/data/raw/master-seed-mix.xlsx
+++ b/data/raw/master-seed-mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BB0CEDC-F36C-4643-A749-1E5E908F71E4}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7029C0B2-BED7-4056-B465-26158824E702}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1100,7 +1100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1141,28 +1141,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>177</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="G2">
         <v>6</v>
       </c>
       <c r="H2">
-        <v>16.25</v>
+        <v>23.52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1170,337 +1170,334 @@
         <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>17.72</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>17.97</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>18.63</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>19.399999999999999</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <v>15.8</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
       <c r="H8">
-        <v>19.899999999999999</v>
+        <v>22.89</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>19.899999999999999</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>20.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>20.5</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H12">
-        <v>21.6</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>21.84</v>
+        <v>23.46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H14">
-        <v>22.5</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H15">
-        <v>23.15</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1508,77 +1505,77 @@
         <v>230</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>11.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>14.2</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="G18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>14.2</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1589,230 +1586,230 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19">
-        <v>15.5</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
-        <v>15.8</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="G21">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H21">
-        <v>15.95</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>16</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
         <v>75</v>
       </c>
       <c r="G23">
-        <v>14</v>
+        <v>1.5</v>
       </c>
       <c r="H23">
-        <v>11.4</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="G24">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H24">
-        <v>11.7</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>219</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G25">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H25">
-        <v>12</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G26">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>12.1</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H27">
-        <v>12.7</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1823,71 +1820,74 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H28">
-        <v>14.2</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>188</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G29">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <v>23.15</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>93</v>
+        <v>209</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G30">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>13.3</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1895,51 +1895,51 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H31">
-        <v>13.7</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="E32" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="G32">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H32">
-        <v>14.2</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1947,77 +1947,77 @@
         <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
         <v>94</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H33">
-        <v>15.5</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>182</v>
       </c>
       <c r="G34">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H34">
-        <v>15.5</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B35" t="s">
         <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>213</v>
       </c>
       <c r="F35" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G35">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H35">
-        <v>15.7</v>
+        <v>23.97</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2025,77 +2025,77 @@
         <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="F36" t="s">
         <v>94</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H36">
-        <v>15.9</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="F37" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G37">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H37">
-        <v>15.1</v>
+        <v>22.87</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H38">
-        <v>16.7</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2106,74 +2106,74 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H39">
-        <v>16.899999999999999</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40">
         <v>12</v>
       </c>
-      <c r="E40" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40">
-        <v>5</v>
-      </c>
       <c r="H40">
-        <v>17</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="E41" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="F41" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H41">
-        <v>17.100000000000001</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2181,25 +2181,25 @@
         <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="F42" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G42">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H42">
-        <v>17.399999999999999</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2207,178 +2207,181 @@
         <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="F43" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G43">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H43">
-        <v>18.100000000000001</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="G44">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>23.38</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="F45" t="s">
         <v>123</v>
       </c>
       <c r="G45">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H45">
-        <v>18.3</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F46" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="G46">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H46">
-        <v>18.7</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="E47" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="F47" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="G47">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H47">
-        <v>19.399999999999999</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="E48" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c r="F48" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="G48">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H48">
-        <v>21.1</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F49" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H49">
-        <v>21.4</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2386,25 +2389,25 @@
         <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="F50" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G50">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H50">
-        <v>21.5</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2412,233 +2415,224 @@
         <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="E51" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="G51">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H51">
-        <v>21.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="F52" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H52">
-        <v>21.6</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="E53" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="G53">
-        <v>2.5</v>
-      </c>
-      <c r="H53">
-        <v>17.97</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="D54" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54">
-        <v>20.25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="E55" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="F55" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="G55">
-        <v>2</v>
-      </c>
-      <c r="H55">
-        <v>19.86</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E56" t="s">
-        <v>42</v>
+        <v>186</v>
       </c>
       <c r="F56" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="G56">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H56">
-        <v>21.84</v>
+        <v>15.97</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="E57" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="G57">
-        <v>0.5</v>
+        <v>9</v>
       </c>
       <c r="H57">
-        <v>21.94</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>155</v>
+        <v>9</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H58">
-        <v>23.31</v>
+        <v>17.72</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="F59" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="G59">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H59">
-        <v>20.25</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -2669,204 +2663,207 @@
         <v>231</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="C61" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="E61" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="F61" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="G61">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="H61">
-        <v>22.5</v>
+        <v>21.94</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s">
-        <v>162</v>
+        <v>32</v>
       </c>
       <c r="E62" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="F62" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="G62">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H62">
-        <v>22.96</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="E63" t="s">
-        <v>166</v>
+        <v>84</v>
       </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="G63">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H63">
-        <v>23.18</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64">
         <v>6</v>
       </c>
-      <c r="C64" t="s">
-        <v>167</v>
-      </c>
-      <c r="D64" t="s">
-        <v>168</v>
-      </c>
-      <c r="E64" t="s">
-        <v>169</v>
-      </c>
-      <c r="F64" t="s">
-        <v>160</v>
-      </c>
-      <c r="G64">
-        <v>2</v>
-      </c>
       <c r="H64">
-        <v>23.33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C65" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>69</v>
       </c>
       <c r="E65" t="s">
-        <v>172</v>
+        <v>93</v>
       </c>
       <c r="F65" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
       <c r="G65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H65">
-        <v>23.38</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="E66" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="F66" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="G66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66">
-        <v>23.38</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>178</v>
+        <v>13</v>
       </c>
       <c r="F67" t="s">
-        <v>160</v>
+        <v>5</v>
       </c>
       <c r="G67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H67">
-        <v>23.52</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
       <c r="C68" t="s">
-        <v>179</v>
+        <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>160</v>
+        <v>104</v>
       </c>
       <c r="G68">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="H68">
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -2877,152 +2874,152 @@
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="F69" t="s">
         <v>182</v>
       </c>
       <c r="G69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H69">
-        <v>13.7</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="D70" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="E70" t="s">
-        <v>4</v>
+        <v>155</v>
       </c>
       <c r="F70" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="G70">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>16.25</v>
+        <v>23.31</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="E71" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="F71" t="s">
-        <v>182</v>
+        <v>75</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H71">
-        <v>16.7</v>
+        <v>20.86</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="E72" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
       <c r="F72" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="H72">
-        <v>17.97</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E73" t="s">
+        <v>99</v>
+      </c>
+      <c r="F73" t="s">
+        <v>94</v>
+      </c>
+      <c r="G73">
         <v>16</v>
       </c>
-      <c r="F73" t="s">
-        <v>182</v>
-      </c>
-      <c r="G73">
-        <v>9</v>
-      </c>
       <c r="H73">
-        <v>18.63</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="C74" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D74" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E74" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="F74" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="G74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H74">
-        <v>19.399999999999999</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -3030,282 +3027,285 @@
         <v>232</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D75" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E75" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F75" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="G75">
         <v>3</v>
       </c>
+      <c r="H75">
+        <v>18.100000000000001</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B76" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="C76" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="D76" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
       <c r="E76" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="F76" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="G76">
-        <v>12</v>
+        <v>2.5</v>
       </c>
       <c r="H76">
-        <v>15.97</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B77" t="s">
         <v>112</v>
       </c>
       <c r="C77" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
-        <v>114</v>
+        <v>215</v>
       </c>
       <c r="E77" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="F77" t="s">
         <v>123</v>
       </c>
       <c r="G77">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H77">
-        <v>18.100000000000001</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="D78" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="E78" t="s">
-        <v>187</v>
+        <v>66</v>
       </c>
       <c r="F78" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="G78">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H78">
-        <v>19.399999999999999</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D79" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="E79" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
       <c r="F79" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G79">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H79">
-        <v>21.1</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B80" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="D80" t="s">
-        <v>135</v>
+        <v>22</v>
       </c>
       <c r="E80" t="s">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="F80" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G80">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H80">
-        <v>21.7</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E81" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F81" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H81">
-        <v>21.84</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="D82" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="E82" t="s">
-        <v>188</v>
+        <v>107</v>
       </c>
       <c r="F82" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G82">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H82">
-        <v>23.15</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D83" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="E83" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F83" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="G83">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H83">
-        <v>19.399999999999999</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D84" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="E84" t="s">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="F84" t="s">
         <v>75</v>
       </c>
       <c r="G84">
-        <v>1.5</v>
+        <v>14</v>
       </c>
       <c r="H84">
-        <v>21.84</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
       <c r="D85" t="s">
-        <v>162</v>
+        <v>35</v>
       </c>
       <c r="E85" t="s">
-        <v>191</v>
+        <v>36</v>
       </c>
       <c r="F85" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="G85">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H85">
-        <v>22.96</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -3313,77 +3313,77 @@
         <v>233</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="C86" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="D86" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="E86" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="F86" t="s">
         <v>75</v>
       </c>
       <c r="G86">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H86">
-        <v>22.89</v>
+        <v>21.66</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B87" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="D87" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="E87" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="F87" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G87">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H87">
-        <v>22.87</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B88" t="s">
         <v>57</v>
       </c>
       <c r="C88" t="s">
-        <v>198</v>
+        <v>134</v>
       </c>
       <c r="D88" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="E88" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="F88" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G88">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H88">
-        <v>21.75</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -3391,51 +3391,51 @@
         <v>233</v>
       </c>
       <c r="B89" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>134</v>
       </c>
       <c r="D89" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="E89" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="F89" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H89">
-        <v>20.86</v>
+        <v>23.83</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B90" t="s">
-        <v>204</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="D90" t="s">
-        <v>206</v>
+        <v>162</v>
       </c>
       <c r="E90" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="F90" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="G90">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H90">
-        <v>21.66</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -3443,181 +3443,181 @@
         <v>233</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C91" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
       <c r="D91" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="E91" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="F91" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G91">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H91">
-        <v>23.46</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C92" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="D92" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="E92" t="s">
-        <v>209</v>
+        <v>88</v>
       </c>
       <c r="F92" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G92">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H92">
-        <v>23.15</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="D93" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
       <c r="E93" t="s">
-        <v>210</v>
+        <v>39</v>
       </c>
       <c r="F93" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H93">
-        <v>23.38</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B94" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>211</v>
+        <v>37</v>
       </c>
       <c r="D94" t="s">
-        <v>212</v>
+        <v>38</v>
       </c>
       <c r="E94" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="F94" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="G94">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H94">
-        <v>23.97</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B95" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>214</v>
+        <v>17</v>
       </c>
       <c r="D95" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
       <c r="E95" t="s">
-        <v>216</v>
+        <v>19</v>
       </c>
       <c r="F95" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G95">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H95">
-        <v>23.5</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B96" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>18</v>
       </c>
       <c r="E96" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="F96" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G96">
         <v>2</v>
       </c>
       <c r="H96">
-        <v>23.83</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="D97" t="s">
-        <v>219</v>
+        <v>18</v>
       </c>
       <c r="E97" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
       <c r="F97" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H97">
-        <v>24.88</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -3628,25 +3628,28 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>221</v>
+        <v>17</v>
       </c>
       <c r="D98" t="s">
-        <v>222</v>
+        <v>18</v>
       </c>
       <c r="E98" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="F98" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G98">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H98">
-        <v>24.2</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H98">
+    <sortCondition ref="C2:C98"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Have gone in circles about these obs that don't have Mix information, not sure if I should take the time to assign them manually or if mix really matters
</commit_message>
<xml_diff>
--- a/data/raw/master-seed-mix.xlsx
+++ b/data/raw/master-seed-mix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7029C0B2-BED7-4056-B465-26158824E702}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09E3E436-8990-450C-81CA-F2A63D39935D}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
@@ -793,10 +793,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1099,8 +1095,8 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add species mix list from Hannah's 2023 publication
</commit_message>
<xml_diff>
--- a/data/raw/master-seed-mix.xlsx
+++ b/data/raw/master-seed-mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09E3E436-8990-450C-81CA-F2A63D39935D}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1E2DDA0-700B-4221-9CD1-4B541CAFD06E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -756,12 +756,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -776,8 +782,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,8 +1102,8 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,28 +1144,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>23.52</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1166,412 +1173,415 @@
         <v>230</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>15.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>15.5</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>20.25</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>20.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>18.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" t="s">
-        <v>194</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8">
+        <v>23.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8">
-        <v>22.89</v>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>18.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>16.25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9" t="s">
-        <v>172</v>
-      </c>
-      <c r="F9" t="s">
-        <v>160</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
       <c r="H9">
-        <v>23.38</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>181</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
+      <c r="H10">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>21.1</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
       <c r="H12">
-        <v>21.1</v>
+        <v>17.72</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>208</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13">
-        <v>23.46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
-      <c r="H14">
-        <v>19.399999999999999</v>
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>187</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>19.399999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+        <v>17.97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="H16">
-        <v>22.5</v>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1">
+        <v>16</v>
+      </c>
+      <c r="H16" s="1">
+        <v>14.2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H17">
-        <v>22.5</v>
+        <v>15.95</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>160</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>23.33</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1579,233 +1589,233 @@
         <v>230</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>21.84</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>21.4</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>21.84</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="H22">
-        <v>21.84</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>190</v>
+        <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G23">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>21.84</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>19.899999999999999</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="D25" t="s">
-        <v>219</v>
+        <v>129</v>
       </c>
       <c r="E25" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="F25" t="s">
         <v>123</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H25">
-        <v>24.88</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>222</v>
+        <v>126</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>127</v>
       </c>
       <c r="F26" t="s">
         <v>123</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H26">
-        <v>24.2</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G27">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>23.15</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1836,54 +1846,54 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G29">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H29">
-        <v>23.15</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="G30">
         <v>3</v>
       </c>
       <c r="H30">
-        <v>23.15</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1891,51 +1901,51 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="G31">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H31">
-        <v>17.100000000000001</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H32">
-        <v>18.63</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1946,74 +1956,74 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H33">
-        <v>15.9</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34">
         <v>15</v>
       </c>
-      <c r="E34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" t="s">
-        <v>182</v>
-      </c>
-      <c r="G34">
-        <v>9</v>
-      </c>
       <c r="H34">
-        <v>18.63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
         <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>211</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>212</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H35">
-        <v>23.97</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2021,77 +2031,71 @@
         <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F36" t="s">
         <v>94</v>
       </c>
       <c r="G36">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H36">
-        <v>15.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="E37" t="s">
-        <v>197</v>
+        <v>92</v>
       </c>
       <c r="F37" t="s">
         <v>75</v>
       </c>
       <c r="G37">
-        <v>4</v>
-      </c>
-      <c r="H37">
-        <v>22.87</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G38">
         <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38">
-        <v>6</v>
-      </c>
-      <c r="H38">
-        <v>16.25</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2102,74 +2106,74 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G39">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H39">
-        <v>15.5</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="G40">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H40">
-        <v>16.25</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="G41">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H41">
-        <v>14.2</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2177,25 +2181,25 @@
         <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E42" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="G42">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H42">
-        <v>14.2</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2203,181 +2207,181 @@
         <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="G43">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H43">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="F44" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H44">
-        <v>23.38</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="E45" t="s">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="F45" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H45">
-        <v>23.38</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F46" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H46">
-        <v>11.5</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="F47" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H47">
-        <v>19.86</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>231</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>72</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>73</v>
       </c>
       <c r="E48" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
       <c r="F48" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H48">
-        <v>23.18</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G49">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H49">
-        <v>19.899999999999999</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2385,25 +2389,25 @@
         <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F50" t="s">
         <v>75</v>
       </c>
       <c r="G50">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H50">
-        <v>11.7</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2411,224 +2415,230 @@
         <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="E51" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="F51" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="G51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H51">
-        <v>13.7</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="E52" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="F52" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52">
-        <v>13.7</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="E53" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="F53" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="G53">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <v>23.52</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B54" t="s">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E54" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F54" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="G54">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>20.25</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B55" t="s">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="D55" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="E55" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="G55">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>20.25</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F56" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="G56">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H56">
-        <v>15.97</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="F57" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="G57">
-        <v>9</v>
-      </c>
-      <c r="H57">
-        <v>21.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="G58">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H58">
-        <v>17.72</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>168</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="F59" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="G59">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H59">
-        <v>17.399999999999999</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -2639,19 +2649,22 @@
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="E60" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="F60" t="s">
         <v>143</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>21.84</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -2659,178 +2672,175 @@
         <v>231</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="E61" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="F61" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="G61">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H61">
-        <v>21.94</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E62" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="F62" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="G62">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H62">
-        <v>20.3</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D63" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="E63" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="F63" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="G63">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H63">
-        <v>12.1</v>
+        <v>23.18</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="E64" t="s">
-        <v>70</v>
+        <v>159</v>
       </c>
       <c r="F64" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="G64">
-        <v>6</v>
-      </c>
-      <c r="H64">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="D65" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="E65" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="F65" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="G65">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="H65">
-        <v>13.3</v>
+        <v>21.94</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="E66" t="s">
-        <v>200</v>
+        <v>155</v>
       </c>
       <c r="F66" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H66">
-        <v>21.75</v>
+        <v>23.31</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="F67" t="s">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="G67">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="H67">
         <v>17.97</v>
@@ -2838,80 +2848,80 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>231</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>162</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F68" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H68">
-        <v>17</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="E69" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F69" t="s">
-        <v>182</v>
+        <v>75</v>
       </c>
       <c r="G69">
         <v>5</v>
       </c>
       <c r="H69">
-        <v>17.97</v>
+        <v>22.89</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="D70" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="F70" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H70">
-        <v>23.31</v>
+        <v>23.46</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -2919,155 +2929,155 @@
         <v>233</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>40</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>41</v>
       </c>
       <c r="E71" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="F71" t="s">
         <v>75</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H71">
-        <v>20.86</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
       <c r="D72" t="s">
-        <v>55</v>
+        <v>219</v>
       </c>
       <c r="E72" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
       <c r="F72" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="G72">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H72">
-        <v>14.2</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>222</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>223</v>
       </c>
       <c r="F73" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G73">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="H73">
-        <v>14.2</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="D74" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="E74" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="F74" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>18.100000000000001</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="C75" t="s">
-        <v>113</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E75" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="F75" t="s">
         <v>123</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H75">
-        <v>18.100000000000001</v>
+        <v>23.97</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B76" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="D76" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="F76" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="G76">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H76">
-        <v>17.97</v>
+        <v>22.87</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -3075,285 +3085,285 @@
         <v>233</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="D77" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="E77" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F77" t="s">
         <v>123</v>
       </c>
       <c r="G77">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H77">
-        <v>23.5</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C78" t="s">
-        <v>64</v>
+        <v>198</v>
       </c>
       <c r="D78" t="s">
-        <v>65</v>
+        <v>199</v>
       </c>
       <c r="E78" t="s">
-        <v>66</v>
+        <v>200</v>
       </c>
       <c r="F78" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="G78">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H78">
-        <v>15.95</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
-        <v>65</v>
+        <v>202</v>
       </c>
       <c r="E79" t="s">
-        <v>66</v>
+        <v>203</v>
       </c>
       <c r="F79" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="G79">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H79">
-        <v>15.1</v>
+        <v>20.86</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B80" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
-        <v>22</v>
+        <v>215</v>
       </c>
       <c r="E80" t="s">
-        <v>23</v>
+        <v>216</v>
       </c>
       <c r="F80" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="G80">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H80">
-        <v>15.8</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="C81" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="D81" t="s">
-        <v>22</v>
+        <v>206</v>
       </c>
       <c r="E81" t="s">
-        <v>23</v>
+        <v>207</v>
       </c>
       <c r="F81" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="G81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H81">
-        <v>15.8</v>
+        <v>21.66</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C82" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="D82" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="E82" t="s">
-        <v>107</v>
+        <v>217</v>
       </c>
       <c r="F82" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="G82">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H82">
-        <v>16.7</v>
+        <v>23.83</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="D83" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
       <c r="E83" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F83" t="s">
-        <v>182</v>
+        <v>75</v>
       </c>
       <c r="G83">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="H83">
-        <v>16.7</v>
+        <v>22.96</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="D84" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="E84" t="s">
-        <v>74</v>
+        <v>189</v>
       </c>
       <c r="F84" t="s">
         <v>75</v>
       </c>
       <c r="G84">
-        <v>14</v>
+        <v>1.5</v>
       </c>
       <c r="H84">
-        <v>11.4</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
       <c r="D85" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="E85" t="s">
-        <v>36</v>
+        <v>130</v>
       </c>
       <c r="F85" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H85">
-        <v>20.5</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B86" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="D86" t="s">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="E86" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="F86" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H86">
-        <v>21.66</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B87" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="D87" t="s">
-        <v>135</v>
+        <v>41</v>
       </c>
       <c r="E87" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="F87" t="s">
         <v>123</v>
       </c>
       <c r="G87">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H87">
-        <v>21.7</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3361,233 +3371,230 @@
         <v>232</v>
       </c>
       <c r="B88" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="D88" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="E88" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="F88" t="s">
         <v>123</v>
       </c>
       <c r="G88">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H88">
-        <v>21.7</v>
+        <v>23.15</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B89" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="E89" t="s">
-        <v>217</v>
+        <v>16</v>
       </c>
       <c r="F89" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="G89">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H89">
-        <v>23.83</v>
+        <v>18.63</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B90" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C90" t="s">
-        <v>161</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="E90" t="s">
-        <v>163</v>
+        <v>4</v>
       </c>
       <c r="F90" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="G90">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H90">
-        <v>22.96</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="D91" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="E91" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
       <c r="F91" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="G91">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H91">
-        <v>22.96</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C92" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D92" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="E92" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="F92" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="G92">
-        <v>4</v>
-      </c>
-      <c r="H92">
-        <v>12.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>37</v>
+        <v>185</v>
       </c>
       <c r="D93" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E93" t="s">
-        <v>39</v>
+        <v>186</v>
       </c>
       <c r="F93" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="G93">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H93">
-        <v>21.6</v>
+        <v>15.97</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D94" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="F94" t="s">
-        <v>138</v>
+        <v>182</v>
       </c>
       <c r="G94">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H94">
-        <v>21.6</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B95" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="C95" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D95" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
       <c r="F95" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="G95">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H95">
-        <v>19.399999999999999</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>71</v>
+        <v>232</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D96" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="E96" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="F96" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="G96">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H96">
-        <v>16.899999999999999</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
@@ -3595,30 +3602,30 @@
         <v>232</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C97" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D97" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="E97" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="F97" t="s">
-        <v>182</v>
+        <v>123</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H97">
-        <v>19.399999999999999</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -3630,21 +3637,21 @@
         <v>18</v>
       </c>
       <c r="E98" t="s">
-        <v>189</v>
+        <v>19</v>
       </c>
       <c r="F98" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
       <c r="G98">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H98">
         <v>19.399999999999999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H98">
-    <sortCondition ref="C2:C98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
+    <sortCondition ref="A1:A99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>